<commit_message>
Intermediate commit to save status
</commit_message>
<xml_diff>
--- a/MotionPlanner/doc/MotionCalculationVisualisation.xlsx
+++ b/MotionPlanner/doc/MotionCalculationVisualisation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="6090" yWindow="900" windowWidth="14400" windowHeight="7245" activeTab="1"/>
+    <workbookView xWindow="6090" yWindow="960" windowWidth="14400" windowHeight="7185" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Parameter" sheetId="5" r:id="rId1"/>
@@ -865,6 +865,10 @@
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
@@ -891,10 +895,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
-      <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1085,7 +1085,7 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>MotionPlanner!$B$14:$B$26</c:f>
+              <c:f>MotionPlanner!$B$13:$B$25</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="13"/>
@@ -1130,45 +1130,45 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>MotionPlanner!$C$14:$C$26</c:f>
+              <c:f>MotionPlanner!$C$13:$C$25</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.83333333333333337</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1.6666666666666667</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>3.3333333333333335</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>4.166666666666667</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>5.833333333333333</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>6.666666666666667</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>7.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>8.3333333333333339</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>9.1666666666666661</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1183,11 +1183,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="110585728"/>
         <c:axId val="112141440"/>
+        <c:axId val="112143360"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="110585728"/>
+        <c:axId val="112141440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1197,12 +1197,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112141440"/>
+        <c:crossAx val="112143360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="112141440"/>
+        <c:axId val="112143360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1213,7 +1213,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110585728"/>
+        <c:crossAx val="112141440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1364,11 +1364,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="127009920"/>
-        <c:axId val="127011456"/>
+        <c:axId val="125707776"/>
+        <c:axId val="125709312"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="127009920"/>
+        <c:axId val="125707776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1378,12 +1378,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="127011456"/>
+        <c:crossAx val="125709312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="127011456"/>
+        <c:axId val="125709312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1394,7 +1394,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="127009920"/>
+        <c:crossAx val="125707776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1609,11 +1609,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="127036800"/>
-        <c:axId val="127038592"/>
+        <c:axId val="137373184"/>
+        <c:axId val="137375104"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="127036800"/>
+        <c:axId val="137373184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1622,7 +1622,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="127038592"/>
+        <c:crossAx val="137375104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1630,7 +1630,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="127038592"/>
+        <c:axId val="137375104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1641,7 +1641,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="127036800"/>
+        <c:crossAx val="137373184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1796,11 +1796,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="132424832"/>
-        <c:axId val="132426368"/>
+        <c:axId val="126787584"/>
+        <c:axId val="126789120"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="132424832"/>
+        <c:axId val="126787584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1810,12 +1810,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="132426368"/>
+        <c:crossAx val="126789120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="132426368"/>
+        <c:axId val="126789120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1826,7 +1826,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="132424832"/>
+        <c:crossAx val="126787584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2032,11 +2032,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="133108864"/>
-        <c:axId val="133110400"/>
+        <c:axId val="127011456"/>
+        <c:axId val="127013248"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="133108864"/>
+        <c:axId val="127011456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2045,7 +2045,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133110400"/>
+        <c:crossAx val="127013248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2053,7 +2053,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="133110400"/>
+        <c:axId val="127013248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2064,7 +2064,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133108864"/>
+        <c:crossAx val="127011456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2097,7 +2097,7 @@
     <xdr:to>
       <xdr:col>22</xdr:col>
       <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>33337</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2170,13 +2170,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2755,10 +2755,10 @@
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:S26"/>
+  <dimension ref="A1:S25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2772,18 +2772,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="16"/>
-      <c r="I1" s="17" t="s">
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="17"/>
+      <c r="I1" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="20"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
@@ -2815,7 +2815,7 @@
         <v>10</v>
       </c>
       <c r="C3" s="9">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D3" s="10">
         <v>0</v>
@@ -2838,7 +2838,7 @@
       </c>
       <c r="C5">
         <f>C3-K2</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D5">
         <f>D3-L2</f>
@@ -2851,7 +2851,7 @@
       </c>
       <c r="B6" s="1">
         <f>SQRT((B5)^2+(C5)^2+(D5)^2)</f>
-        <v>10</v>
+        <v>14.142135623730951</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
@@ -2868,7 +2868,7 @@
       </c>
       <c r="B8" s="1">
         <f>B6/B2/B7</f>
-        <v>0.41666666666666669</v>
+        <v>0.58925565098878963</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
@@ -2876,11 +2876,11 @@
       <c r="B9" s="1"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="J10" s="13" t="s">
+      <c r="J10" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
@@ -2892,10 +2892,10 @@
       <c r="D11" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G11" s="13" t="s">
+      <c r="G11" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="H11" s="13"/>
+      <c r="H11" s="14"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2" t="s">
         <v>23</v>
@@ -2911,60 +2911,88 @@
       <c r="S11" s="2"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
+      <c r="A12">
+        <v>0</v>
+      </c>
+      <c r="B12" s="13">
+        <f>J2</f>
+        <v>0</v>
+      </c>
+      <c r="C12" s="13">
+        <f>K2</f>
+        <v>0</v>
+      </c>
+      <c r="D12" s="13">
+        <f>L2</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>0</v>
-      </c>
-      <c r="B13" s="20">
-        <f>J2</f>
-        <v>0</v>
-      </c>
-      <c r="C13" s="20">
-        <f>K2</f>
-        <v>0</v>
-      </c>
-      <c r="D13" s="20">
-        <f>L2</f>
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="B13" s="1">
+        <f>$J$2+$B$5*A13/$B$7</f>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="C13" s="1">
+        <f>$K$2+$C$5*A13/$B$7</f>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="D13" s="1">
+        <f>$L$2+$D$5*A13/$B$7</f>
+        <v>0</v>
+      </c>
+      <c r="J13" s="1">
+        <f>SQRT(Parameter!$B$5 - (Parameter!$B$6-$J$2+B13)^2 - (Parameter!$B$7-$K$2+C13)^2)+$L$2+D13</f>
+        <v>122.87155379601268</v>
+      </c>
+      <c r="M13" s="1"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B14" s="1">
         <f>$J$2+$B$5*A14/$B$7</f>
-        <v>0.83333333333333337</v>
+        <v>1.6666666666666667</v>
       </c>
       <c r="C14" s="1">
         <f>$K$2+$C$5*A14/$B$7</f>
-        <v>0</v>
+        <v>1.6666666666666667</v>
       </c>
       <c r="D14" s="1">
         <f>$L$2+$D$5*A14/$B$7</f>
         <v>0</v>
       </c>
+      <c r="I14" s="1"/>
       <c r="J14" s="1">
         <f>SQRT(Parameter!$B$5 - (Parameter!$B$6-$J$2+B14)^2 - (Parameter!$B$7-$K$2+C14)^2)+$L$2+D14</f>
-        <v>122.26247656861399</v>
+        <v>124.5112833710869</v>
+      </c>
+      <c r="K14" s="12">
+        <f t="shared" ref="K14:K24" si="0">J14-J13</f>
+        <v>1.6397295750742273</v>
+      </c>
+      <c r="L14" s="1">
+        <f t="shared" ref="L14:L24" si="1">K14/$B$8</f>
+        <v>2.7827133644330933</v>
       </c>
       <c r="M14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B15" s="1">
         <f>$J$2+$B$5*A15/$B$7</f>
-        <v>1.6666666666666667</v>
+        <v>2.5</v>
       </c>
       <c r="C15" s="1">
         <f>$K$2+$C$5*A15/$B$7</f>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="D15" s="1">
         <f>$L$2+$D$5*A15/$B$7</f>
@@ -2973,15 +3001,15 @@
       <c r="I15" s="1"/>
       <c r="J15" s="1">
         <f>SQRT(Parameter!$B$5 - (Parameter!$B$6-$J$2+B15)^2 - (Parameter!$B$7-$K$2+C15)^2)+$L$2+D15</f>
-        <v>123.31195183149474</v>
-      </c>
-      <c r="K15" s="12">
-        <f>J15-J14</f>
-        <v>1.0494752628807476</v>
+        <v>126.11868562352682</v>
+      </c>
+      <c r="K15" s="1">
+        <f t="shared" si="0"/>
+        <v>1.6074022524399112</v>
       </c>
       <c r="L15" s="1">
-        <f>K15/$B$8</f>
-        <v>2.5187406309137939</v>
+        <f t="shared" si="1"/>
+        <v>2.7278520787075005</v>
       </c>
       <c r="M15" s="1"/>
       <c r="R15" s="1"/>
@@ -2989,15 +3017,15 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B16" s="1">
         <f>$J$2+$B$5*A16/$B$7</f>
-        <v>2.5</v>
+        <v>3.3333333333333335</v>
       </c>
       <c r="C16" s="1">
         <f>$K$2+$C$5*A16/$B$7</f>
-        <v>0</v>
+        <v>3.3333333333333335</v>
       </c>
       <c r="D16" s="1">
         <f>$L$2+$D$5*A16/$B$7</f>
@@ -3006,15 +3034,15 @@
       <c r="I16" s="1"/>
       <c r="J16" s="1">
         <f>SQRT(Parameter!$B$5 - (Parameter!$B$6-$J$2+B16)^2 - (Parameter!$B$7-$K$2+C16)^2)+$L$2+D16</f>
-        <v>124.34698574314534</v>
+        <v>127.69498135134013</v>
       </c>
       <c r="K16" s="1">
-        <f>J16-J15</f>
-        <v>1.0350339116506007</v>
+        <f t="shared" si="0"/>
+        <v>1.5762957278133172</v>
       </c>
       <c r="L16" s="1">
-        <f>K16/$B$8</f>
-        <v>2.4840813879614414</v>
+        <f t="shared" si="1"/>
+        <v>2.675062555901234</v>
       </c>
       <c r="M16" s="1"/>
       <c r="R16" s="1"/>
@@ -3022,15 +3050,15 @@
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B17" s="1">
         <f>$J$2+$B$5*A17/$B$7</f>
-        <v>3.3333333333333335</v>
+        <v>4.166666666666667</v>
       </c>
       <c r="C17" s="1">
         <f>$K$2+$C$5*A17/$B$7</f>
-        <v>0</v>
+        <v>4.166666666666667</v>
       </c>
       <c r="D17" s="1">
         <f>$L$2+$D$5*A17/$B$7</f>
@@ -3039,15 +3067,15 @@
       <c r="I17" s="1"/>
       <c r="J17" s="1">
         <f>SQRT(Parameter!$B$5 - (Parameter!$B$6-$J$2+B17)^2 - (Parameter!$B$7-$K$2+C17)^2)+$L$2+D17</f>
-        <v>125.36793598616121</v>
+        <v>129.24130873468602</v>
       </c>
       <c r="K17" s="1">
-        <f>J17-J16</f>
-        <v>1.020950243015875</v>
+        <f t="shared" si="0"/>
+        <v>1.5463273833458828</v>
       </c>
       <c r="L17" s="1">
-        <f>K17/$B$8</f>
-        <v>2.4502805832380998</v>
+        <f t="shared" si="1"/>
+        <v>2.6242045888759771</v>
       </c>
       <c r="M17" s="1"/>
       <c r="R17" s="1"/>
@@ -3055,15 +3083,15 @@
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B18" s="1">
         <f>$J$2+$B$5*A18/$B$7</f>
-        <v>4.166666666666667</v>
+        <v>5</v>
       </c>
       <c r="C18" s="1">
         <f>$K$2+$C$5*A18/$B$7</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D18" s="1">
         <f>$L$2+$D$5*A18/$B$7</f>
@@ -3072,15 +3100,15 @@
       <c r="I18" s="1"/>
       <c r="J18" s="1">
         <f>SQRT(Parameter!$B$5 - (Parameter!$B$6-$J$2+B18)^2 - (Parameter!$B$7-$K$2+C18)^2)+$L$2+D18</f>
-        <v>126.37514389533069</v>
+        <v>130.75873097736911</v>
       </c>
       <c r="K18" s="1">
-        <f>J18-J17</f>
-        <v>1.0072079091694803</v>
+        <f t="shared" si="0"/>
+        <v>1.5174222426830966</v>
       </c>
       <c r="L18" s="1">
-        <f>K18/$B$8</f>
-        <v>2.4172989820067525</v>
+        <f t="shared" si="1"/>
+        <v>2.5751509385388398</v>
       </c>
       <c r="M18" s="1"/>
       <c r="R18" s="1"/>
@@ -3088,15 +3116,15 @@
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B19" s="1">
         <f>$J$2+$B$5*A19/$B$7</f>
-        <v>5</v>
+        <v>5.833333333333333</v>
       </c>
       <c r="C19" s="1">
         <f>$K$2+$C$5*A19/$B$7</f>
-        <v>0</v>
+        <v>5.833333333333333</v>
       </c>
       <c r="D19" s="1">
         <f>$L$2+$D$5*A19/$B$7</f>
@@ -3105,15 +3133,15 @@
       <c r="I19" s="1"/>
       <c r="J19" s="1">
         <f>SQRT(Parameter!$B$5 - (Parameter!$B$6-$J$2+B19)^2 - (Parameter!$B$7-$K$2+C19)^2)+$L$2+D19</f>
-        <v>127.36893548590247</v>
+        <v>132.24824305975397</v>
       </c>
       <c r="K19" s="1">
-        <f>J19-J18</f>
-        <v>0.99379159057177446</v>
+        <f t="shared" si="0"/>
+        <v>1.4895120823848629</v>
       </c>
       <c r="L19" s="1">
-        <f>K19/$B$8</f>
-        <v>2.3850998173722586</v>
+        <f t="shared" si="1"/>
+        <v>2.5277858258727166</v>
       </c>
       <c r="M19" s="1"/>
       <c r="R19" s="1"/>
@@ -3121,15 +3149,15 @@
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B20" s="1">
         <f>$J$2+$B$5*A20/$B$7</f>
-        <v>5.833333333333333</v>
+        <v>6.666666666666667</v>
       </c>
       <c r="C20" s="1">
         <f>$K$2+$C$5*A20/$B$7</f>
-        <v>0</v>
+        <v>6.666666666666667</v>
       </c>
       <c r="D20" s="1">
         <f>$L$2+$D$5*A20/$B$7</f>
@@ -3138,15 +3166,15 @@
       <c r="I20" s="1"/>
       <c r="J20" s="1">
         <f>SQRT(Parameter!$B$5 - (Parameter!$B$6-$J$2+B20)^2 - (Parameter!$B$7-$K$2+C20)^2)+$L$2+D20</f>
-        <v>128.34962239979336</v>
+        <v>133.71077772638137</v>
       </c>
       <c r="K20" s="1">
-        <f>J20-J19</f>
-        <v>0.98068691389089224</v>
+        <f t="shared" si="0"/>
+        <v>1.4625346666273913</v>
       </c>
       <c r="L20" s="1">
-        <f>K20/$B$8</f>
-        <v>2.3536485933381415</v>
+        <f t="shared" si="1"/>
+        <v>2.4820036331823241</v>
       </c>
       <c r="M20" s="1"/>
       <c r="R20" s="1"/>
@@ -3154,15 +3182,15 @@
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B21" s="1">
         <f>$J$2+$B$5*A21/$B$7</f>
-        <v>6.666666666666667</v>
+        <v>7.5</v>
       </c>
       <c r="C21" s="1">
         <f>$K$2+$C$5*A21/$B$7</f>
-        <v>0</v>
+        <v>7.5</v>
       </c>
       <c r="D21" s="1">
         <f>$L$2+$D$5*A21/$B$7</f>
@@ -3171,15 +3199,15 @@
       <c r="I21" s="1"/>
       <c r="J21" s="1">
         <f>SQRT(Parameter!$B$5 - (Parameter!$B$6-$J$2+B21)^2 - (Parameter!$B$7-$K$2+C21)^2)+$L$2+D21</f>
-        <v>129.31750277761398</v>
+        <v>135.14721081183282</v>
       </c>
       <c r="K21" s="1">
-        <f>J21-J20</f>
-        <v>0.9678803778206202</v>
+        <f t="shared" si="0"/>
+        <v>1.4364330854514549</v>
       </c>
       <c r="L21" s="1">
-        <f>K21/$B$8</f>
-        <v>2.3229129067694885</v>
+        <f t="shared" si="1"/>
+        <v>2.4377077810642542</v>
       </c>
       <c r="M21" s="1"/>
       <c r="R21" s="1"/>
@@ -3187,15 +3215,15 @@
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B22" s="1">
         <f>$J$2+$B$5*A22/$B$7</f>
-        <v>7.5</v>
+        <v>8.3333333333333339</v>
       </c>
       <c r="C22" s="1">
         <f>$K$2+$C$5*A22/$B$7</f>
-        <v>0</v>
+        <v>8.3333333333333339</v>
       </c>
       <c r="D22" s="1">
         <f>$L$2+$D$5*A22/$B$7</f>
@@ -3204,15 +3232,15 @@
       <c r="I22" s="1"/>
       <c r="J22" s="1">
         <f>SQRT(Parameter!$B$5 - (Parameter!$B$6-$J$2+B22)^2 - (Parameter!$B$7-$K$2+C22)^2)+$L$2+D22</f>
-        <v>130.27286206350877</v>
+        <v>136.55836599221749</v>
       </c>
       <c r="K22" s="1">
-        <f>J22-J21</f>
-        <v>0.95535928589478658</v>
+        <f t="shared" si="0"/>
+        <v>1.411155180384668</v>
       </c>
       <c r="L22" s="1">
-        <f>K22/$B$8</f>
-        <v>2.2928622861474879</v>
+        <f t="shared" si="1"/>
+        <v>2.3948097536556587</v>
       </c>
       <c r="M22" s="1"/>
       <c r="R22" s="1"/>
@@ -3220,15 +3248,15 @@
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B23" s="1">
         <f>$J$2+$B$5*A23/$B$7</f>
-        <v>8.3333333333333339</v>
+        <v>9.1666666666666661</v>
       </c>
       <c r="C23" s="1">
         <f>$K$2+$C$5*A23/$B$7</f>
-        <v>0</v>
+        <v>9.1666666666666661</v>
       </c>
       <c r="D23" s="1">
         <f>$L$2+$D$5*A23/$B$7</f>
@@ -3237,15 +3265,15 @@
       <c r="I23" s="1"/>
       <c r="J23" s="1">
         <f>SQRT(Parameter!$B$5 - (Parameter!$B$6-$J$2+B23)^2 - (Parameter!$B$7-$K$2+C23)^2)+$L$2+D23</f>
-        <v>131.21597374904044</v>
+        <v>137.94501903632869</v>
       </c>
       <c r="K23" s="1">
-        <f>J23-J22</f>
-        <v>0.9431116855316759</v>
+        <f t="shared" si="0"/>
+        <v>1.3866530441111991</v>
       </c>
       <c r="L23" s="1">
-        <f>K23/$B$8</f>
-        <v>2.2634680452760221</v>
+        <f t="shared" si="1"/>
+        <v>2.3532282495455945</v>
       </c>
       <c r="M23" s="1"/>
       <c r="R23" s="1"/>
@@ -3253,15 +3281,15 @@
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B24" s="1">
         <f>$J$2+$B$5*A24/$B$7</f>
-        <v>9.1666666666666661</v>
+        <v>10</v>
       </c>
       <c r="C24" s="1">
         <f>$K$2+$C$5*A24/$B$7</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D24" s="1">
         <f>$L$2+$D$5*A24/$B$7</f>
@@ -3270,67 +3298,34 @@
       <c r="I24" s="1"/>
       <c r="J24" s="1">
         <f>SQRT(Parameter!$B$5 - (Parameter!$B$6-$J$2+B24)^2 - (Parameter!$B$7-$K$2+C24)^2)+$L$2+D24</f>
-        <v>132.14710006167695</v>
+        <v>139.30790161948451</v>
       </c>
       <c r="K24" s="1">
-        <f>J24-J23</f>
-        <v>0.93112631263650769</v>
+        <f t="shared" si="0"/>
+        <v>1.3628825831558231</v>
       </c>
       <c r="L24" s="1">
-        <f>K24/$B$8</f>
-        <v>2.2347031503276185</v>
+        <f t="shared" si="1"/>
+        <v>2.3128884396252509</v>
       </c>
       <c r="M24" s="1"/>
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>12</v>
-      </c>
-      <c r="B25" s="1">
-        <f>$J$2+$B$5*A25/$B$7</f>
-        <v>10</v>
-      </c>
-      <c r="C25" s="1">
-        <f>$K$2+$C$5*A25/$B$7</f>
-        <v>0</v>
-      </c>
-      <c r="D25" s="1">
-        <f>$L$2+$D$5*A25/$B$7</f>
-        <v>0</v>
-      </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
       <c r="I25" s="1"/>
-      <c r="J25" s="1">
-        <f>SQRT(Parameter!$B$5 - (Parameter!$B$6-$J$2+B25)^2 - (Parameter!$B$7-$K$2+C25)^2)+$L$2+D25</f>
-        <v>133.06649260284865</v>
-      </c>
-      <c r="K25" s="1">
-        <f>J25-J24</f>
-        <v>0.91939254117170321</v>
-      </c>
-      <c r="L25" s="1">
-        <f>K25/$B$8</f>
-        <v>2.2065420988120876</v>
-      </c>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
       <c r="M25" s="1"/>
-      <c r="R25" s="1"/>
-      <c r="S25" s="1"/>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
-      <c r="M26" s="1"/>
-      <c r="O26" s="1"/>
-      <c r="P26" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>